<commit_message>
Reduce WHO Pertussis from 5-dose to 4-dose (3p+1) per WHO guidance
WHO does not recommend a school-entry booster (dose 5). Series is now
3 primary doses at 6/10/14 weeks plus 1 booster at 12-23 months.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cicada_generator/lib/WHO/antigen/Pertussis.xlsx
+++ b/cicada_generator/lib/WHO/antigen/Pertussis.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="5-dose series" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="4-dose series" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
   <si>
-    <t xml:space="preserve">WHO Pertussis 5-dose series</t>
+    <t xml:space="preserve">WHO Pertussis 4-dose series (3p+1)</t>
   </si>
   <si>
     <t xml:space="preserve">Target Disease</t>
@@ -132,18 +132,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tdap (115)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 years</t>
   </si>
 </sst>
 </file>
@@ -500,12 +488,6 @@
       <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -621,12 +603,6 @@
       <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
@@ -656,15 +632,6 @@
       <c r="I17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
@@ -780,12 +747,6 @@
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
@@ -815,15 +776,6 @@
       <c r="I26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
@@ -939,12 +891,6 @@
       <c r="F34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
@@ -974,15 +920,6 @@
       <c r="I35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
@@ -1077,174 +1014,6 @@
         <v>27</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>